<commit_message>
trabalho 07 - Bellman-Ford
</commit_message>
<xml_diff>
--- a/docs/Grafos/grafoII.xlsx
+++ b/docs/Grafos/grafoII.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiago\Documents\Cience Computing\Unifor\Trabalhos\Resolução de problemas com grafos\grafosPy\docs\Grafos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48015E1-004A-40B5-B24B-5C31E8F3613E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="grafo1"/>
-    <sheet r:id="rId2" sheetId="2" name="grafo2"/>
-    <sheet r:id="rId3" sheetId="3" name="grafo3"/>
+    <sheet name="grafo1" sheetId="1" r:id="rId1"/>
+    <sheet name="grafo2" sheetId="2" r:id="rId2"/>
+    <sheet name="grafo3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -84,8 +90,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -121,7 +126,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffd966"/>
+        <fgColor rgb="FFFFD966"/>
       </patternFill>
     </fill>
   </fills>
@@ -157,16 +162,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -175,61 +180,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -240,10 +246,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
@@ -281,71 +287,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -373,7 +379,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -396,11 +402,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -409,13 +415,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -425,7 +431,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -434,7 +440,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -443,7 +449,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -451,10 +457,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -519,7 +525,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -529,17 +535,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="15" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="14.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="14.140625" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row r="1" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -565,7 +565,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
+    <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>7</v>
       </c>
@@ -591,7 +591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
+    <row r="3" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>8</v>
       </c>
@@ -617,7 +617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
+    <row r="4" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>9</v>
       </c>
@@ -643,7 +643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
+    <row r="5" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>10</v>
       </c>
@@ -669,7 +669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
+    <row r="6" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>11</v>
       </c>
@@ -695,7 +695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
+    <row r="7" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>12</v>
       </c>
@@ -721,7 +721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
+    <row r="8" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>13</v>
       </c>
@@ -753,34 +753,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="14.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="15" width="14.140625" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -827,7 +816,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
@@ -844,10 +833,10 @@
         <v>0</v>
       </c>
       <c r="F2" s="8">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G2" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" s="8">
         <v>0</v>
@@ -865,7 +854,7 @@
         <v>0</v>
       </c>
       <c r="M2" s="8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N2" s="8">
         <v>0</v>
@@ -874,7 +863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row r="3" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
@@ -885,13 +874,13 @@
         <v>0</v>
       </c>
       <c r="D3" s="8">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E3" s="8">
         <v>0</v>
       </c>
       <c r="F3" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" s="8">
         <v>0</v>
@@ -903,7 +892,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="8">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K3" s="8">
         <v>0</v>
@@ -921,7 +910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row r="4" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
@@ -935,7 +924,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F4" s="8">
         <v>0</v>
@@ -944,7 +933,7 @@
         <v>3</v>
       </c>
       <c r="H4" s="8">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I4" s="8">
         <v>0</v>
@@ -953,7 +942,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="8">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L4" s="8">
         <v>0</v>
@@ -968,7 +957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row r="5" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -991,7 +980,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I5" s="8">
         <v>0</v>
@@ -1012,10 +1001,10 @@
         <v>0</v>
       </c>
       <c r="O5" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>11</v>
       </c>
@@ -1062,7 +1051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row r="7" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
@@ -1085,13 +1074,13 @@
         <v>0</v>
       </c>
       <c r="H7" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="8">
         <v>0</v>
       </c>
       <c r="J7" s="8">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K7" s="8">
         <v>0</v>
@@ -1103,13 +1092,13 @@
         <v>0</v>
       </c>
       <c r="N7" s="8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O7" s="8">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row r="8" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>13</v>
       </c>
@@ -1156,7 +1145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row r="9" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>14</v>
       </c>
@@ -1185,7 +1174,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K9" s="8">
         <v>0</v>
@@ -1197,13 +1186,13 @@
         <v>0</v>
       </c>
       <c r="N9" s="8">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="O9" s="8">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row r="10" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>15</v>
       </c>
@@ -1250,7 +1239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row r="11" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>16</v>
       </c>
@@ -1285,10 +1274,10 @@
         <v>0</v>
       </c>
       <c r="L11" s="8">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="M11" s="8">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="N11" s="8">
         <v>0</v>
@@ -1297,7 +1286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row r="12" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>17</v>
       </c>
@@ -1338,13 +1327,13 @@
         <v>0</v>
       </c>
       <c r="N12" s="8">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="O12" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>18</v>
       </c>
@@ -1391,7 +1380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row r="14" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>19</v>
       </c>
@@ -1438,7 +1427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row r="15" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>20</v>
       </c>
@@ -1487,30 +1476,26 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="4" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="14.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="14.140625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1533,7 +1518,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1556,7 +1541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row r="3" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1579,7 +1564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1602,7 +1587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row r="5" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1625,7 +1610,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row r="6" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1648,7 +1633,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row r="7" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>

</xml_diff>